<commit_message>
Gerbers Generated and Buzzer Interface Added
</commit_message>
<xml_diff>
--- a/V1R0/HARDWARE/Secadora Filamentos.xlsx
+++ b/V1R0/HARDWARE/Secadora Filamentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects_Git\filament_dryer\V1R0\HARDWARE\Project Outputs for Secadora Filamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA9A68D2-7DB4-41CB-A1A1-2ECE289FD414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAEC62A2-AE02-41D8-9B2B-2B1729ADFD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="11170" xr2:uid="{C9E740B8-895E-43E1-9C91-B78BE2499338}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="11170" firstSheet="1" activeTab="1" xr2:uid="{C9E740B8-895E-43E1-9C91-B78BE2499338}"/>
   </bookViews>
   <sheets>
     <sheet name="Secadora Filamentos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>61301011821</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>Opto Triac 400VDRM 10mA</t>
+  </si>
+  <si>
+    <t>14230226011</t>
+  </si>
+  <si>
+    <t>140816140410</t>
   </si>
 </sst>
 </file>
@@ -423,14 +435,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -750,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8ECD26-3201-4846-B4C4-CE3E0BE83990}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -860,7 +870,7 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -880,7 +890,7 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -920,7 +930,7 @@
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1257,7 +1267,7 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -1337,7 +1347,7 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="6" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1362,10 +1372,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1">
-      <c r="F32" s="7"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="3:3" ht="15" customHeight="1">
-      <c r="C33" s="7"/>
+      <c r="C33" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{8D8ECD26-3201-4846-B4C4-CE3E0BE83990}"/>
@@ -1379,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF92D1F4-F2B3-4831-A31F-982A03DB0833}">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1458,7 +1468,7 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1475,7 +1485,7 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1562,6 +1572,40 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="1">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>